<commit_message>
log_maker file and logs directory
</commit_message>
<xml_diff>
--- a/excel_files/Libro1.xlsx
+++ b/excel_files/Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmver\Documents\developments\santander\script-excel-to-sqlerver\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB73B1F-BCF4-4E5E-ABF1-B6692656B827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C044FAC5-DFBB-4B42-ABF0-AF70AE62F61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="1755" windowWidth="28800" windowHeight="15885" xr2:uid="{3BDD47B2-EB73-42BA-85E4-C285045AD002}"/>
+    <workbookView xWindow="4560" yWindow="1815" windowWidth="20910" windowHeight="11835" xr2:uid="{3BDD47B2-EB73-42BA-85E4-C285045AD002}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>